<commit_message>
# Reading of config from `config.json` and reading of area fraction values
</commit_message>
<xml_diff>
--- a/Wafer Mapping.xlsx
+++ b/Wafer Mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gohja\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gohja\Desktop\wafer-map-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887C14FF-A198-4F9C-8188-3D50FF8F3032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CFC483-0802-4E64-B2B1-A24AD1DFB7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="532" firstSheet="11" activeTab="12" xr2:uid="{FA4B9650-7B02-4CC5-8F9C-DDE85E2BCFF1}"/>
   </bookViews>
@@ -41965,7 +41965,7 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:C50"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>